<commit_message>
Sales Analysis with the possibility of setting up a truck with fish load for each city
</commit_message>
<xml_diff>
--- a/Sales Analysis.xlsx
+++ b/Sales Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Quark Projects\Katas\Lonja Kata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED755C1A-3E47-4217-BB0D-57DD8C705579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D90A144-01A5-4E22-AA59-D07F0F873B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0C5F48C-189D-49E4-B0A9-DAB01DE01715}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Vieiras</t>
   </si>
@@ -53,18 +53,12 @@
     <t>Lisboa</t>
   </si>
   <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
     <t>Ventas</t>
   </si>
   <si>
     <t>$/kg</t>
   </si>
   <si>
-    <t>Venta</t>
-  </si>
-  <si>
     <t>Distancia</t>
   </si>
   <si>
@@ -75,6 +69,9 @@
   </si>
   <si>
     <t>Beneficio</t>
+  </si>
+  <si>
+    <t>Destino/pescado</t>
   </si>
 </sst>
 </file>
@@ -435,20 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1ACA5F2-77FE-49B1-AF7B-FC5073E90BF1}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -460,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +471,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -488,7 +485,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -502,62 +499,86 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>100</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -569,50 +590,50 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12">
-        <f>$B7*$B2</f>
-        <v>25000</v>
+        <f>B7*B2</f>
+        <v>0</v>
       </c>
       <c r="C12">
-        <f>$B7*$C2</f>
-        <v>22500</v>
+        <f t="shared" ref="C12:D12" si="0">C7*C2</f>
+        <v>0</v>
       </c>
       <c r="D12">
-        <f>$B7*$D2</f>
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:D14" si="0">$B8*$B3</f>
+        <f t="shared" ref="B13:D13" si="1">B8*B3</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C14" si="1">$B8*$C3</f>
-        <v>12000</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D14" si="2">$B8*$D3</f>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>22500</v>
+        <f t="shared" ref="B14:D14" si="2">B9*B4</f>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D14">
@@ -620,54 +641,58 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f>-IF(SUM(B12:B14)&gt;0,5+2*$G$7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>-IF(SUM(C12:C14)&gt;0,5+2*$G$8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>-IF(SUM(D12:D14)&gt;0,5+2*$G$9,0)</f>
+        <v>-1205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>-SUM(B12:B14)*G7/100*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>-SUM(C12:C14)*G8/100*0.01</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>-SUM(D12:D14)*G9/100*0.01</f>
+        <v>-3900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
-      </c>
-      <c r="B15">
-        <f>-IF(SUM(B12:B14)&gt;0,5+2*$E$7,0)</f>
-        <v>-1605</v>
-      </c>
-      <c r="C15">
-        <f>-IF(SUM(C12:C14)&gt;0,5+2*$E$8,0)</f>
-        <v>-2205</v>
-      </c>
-      <c r="D15">
-        <f>-IF(SUM(D12:D14)&gt;0,5+2*$E$9,0)</f>
-        <v>-1205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <f>-SUM(B12:B14)*E7/100*0.01</f>
-        <v>-3800</v>
-      </c>
-      <c r="C16">
-        <f>-SUM(C12:C14)*E8/100*0.01</f>
-        <v>-3795</v>
-      </c>
-      <c r="D16">
-        <f>-SUM(D12:D14)*E9/100*0.01</f>
-        <v>-3900</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
       </c>
       <c r="B17">
         <f>SUM(B12:B16)</f>
-        <v>42095</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:D17" si="3">SUM(C12:C16)</f>
-        <v>28500</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
+        <v>59895</v>
+      </c>
+      <c r="E17">
+        <f>SUM(B17:D17)</f>
         <v>59895</v>
       </c>
     </row>

</xml_diff>